<commit_message>
added final backend with jwt auth requirement for analyzing
</commit_message>
<xml_diff>
--- a/App/data/starter_bioremediation_kinetics_dataset.xlsx
+++ b/App/data/starter_bioremediation_kinetics_dataset.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vivek\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA37BBC-3724-4B0A-9940-27A85E253489}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>Pollutant</t>
   </si>
@@ -95,13 +101,28 @@
   </si>
   <si>
     <t>Frontiers crude oil kinetics study</t>
+  </si>
+  <si>
+    <t>LDPE</t>
+  </si>
+  <si>
+    <t>Aspergillus</t>
+  </si>
+  <si>
+    <t>Ahmed et al. 2025 (LDPE weight loss); fungal dye kinetic studies</t>
+  </si>
+  <si>
+    <t>Escherichia coli</t>
+  </si>
+  <si>
+    <t>Sokół 1988; Haldane fits for phenol degradation by E. coli and Pseudomonas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -164,13 +185,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -208,7 +237,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -242,6 +271,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -276,9 +306,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -451,14 +482,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="13.44140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -493,7 +529,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -528,7 +564,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -563,7 +599,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -577,7 +613,7 @@
         <v>8</v>
       </c>
       <c r="E4">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F4">
         <v>300</v>
@@ -598,7 +634,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -633,7 +669,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -668,7 +704,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -682,7 +718,7 @@
         <v>12</v>
       </c>
       <c r="E7">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="F7">
         <v>1000</v>
@@ -694,13 +730,83 @@
         <v>250</v>
       </c>
       <c r="I7">
-        <v>16.9</v>
+        <v>16.899999999999999</v>
       </c>
       <c r="J7">
         <v>4.5</v>
       </c>
       <c r="K7" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8">
+        <v>30</v>
+      </c>
+      <c r="D8">
+        <v>80</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>150</v>
+      </c>
+      <c r="G8">
+        <v>5</v>
+      </c>
+      <c r="H8">
+        <v>200</v>
+      </c>
+      <c r="I8">
+        <v>0.12</v>
+      </c>
+      <c r="J8">
+        <v>50</v>
+      </c>
+      <c r="K8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9">
+        <v>30</v>
+      </c>
+      <c r="D9">
+        <v>4</v>
+      </c>
+      <c r="E9">
+        <v>1.9</v>
+      </c>
+      <c r="F9">
+        <v>200</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>500</v>
+      </c>
+      <c r="I9">
+        <v>0.25</v>
+      </c>
+      <c r="J9">
+        <v>45</v>
+      </c>
+      <c r="K9" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>